<commit_message>
REFACTOR:Rename folder to baseCode->baseCodeGui
</commit_message>
<xml_diff>
--- a/WBS.xlsx
+++ b/WBS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gimminseo/wumpusWorld/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC569A3E-3FA2-2F4C-8955-24298F54BAA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A165AF-F882-084E-B657-047DF3DB061C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{BB78278F-2B75-4149-889F-758E33B0EEC8}"/>
   </bookViews>
@@ -177,17 +177,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -509,7 +509,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -532,51 +532,51 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1"/>
+      <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1"/>
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1"/>
+      <c r="A5" s="4"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1"/>
+      <c r="A6" s="4"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1"/>
+      <c r="A7" s="4"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1"/>
+      <c r="A8" s="4"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1"/>
+      <c r="A9" s="4"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1"/>
+      <c r="A10" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>